<commit_message>
se solucionaron funciones trucadas
</commit_message>
<xml_diff>
--- a/2024-12-13.xlsx
+++ b/2024-12-13.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>S107</t>
+          <t>S111</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>S112</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>S110</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>S109</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>S108</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego la funcion de imprimir el codigo y la hora exacta de registro
</commit_message>
<xml_diff>
--- a/2024-12-13.xlsx
+++ b/2024-12-13.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,27 +443,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>S111</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>S112</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>S110</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>S109</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>S108</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
sig:enlazar los codigos a un usuario en especifico con su informacion personal
</commit_message>
<xml_diff>
--- a/2024-12-13.xlsx
+++ b/2024-12-13.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>S108</t>
+          <t>S112</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>S110</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>S109</t>
         </is>
       </c>
     </row>

</xml_diff>